<commit_message>
Added bandCreatorResponse, but need fix
</commit_message>
<xml_diff>
--- a/Bands.xlsx
+++ b/Bands.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>ЖЕКА РАСТУ (Кто там?)</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>rate</t>
+  </si>
+  <si>
+    <t>Genre</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +472,7 @@
     <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -485,8 +488,11 @@
       <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -497,7 +503,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -508,7 +514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -519,7 +525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -530,7 +536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -541,7 +547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -552,7 +558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -563,7 +569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -574,7 +580,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -585,7 +591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -596,7 +602,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -607,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -618,7 +624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -629,7 +635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -640,7 +646,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>

</xml_diff>